<commit_message>
[honda.xlsx] drop platform overrides
</commit_message>
<xml_diff>
--- a/src/test/resources/excelData/Honda/honda.xlsx
+++ b/src/test/resources/excelData/Honda/honda.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\New\SeleniumFramework\src\test\resources\excelData\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\EclipseWorkspace\SeleniumFramework\src\test\resources\excelData\Honda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705BC52F-22B4-414C-AC28-F67CF3027115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42372568-887B-4654-A239-7E460EE7AED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{506A9C37-F3E9-44B3-8F46-074FAF0AE875}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>TestMethodName</t>
   </si>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t>desktopIe</t>
-  </si>
-  <si>
-    <t>AndroidChromeTest2</t>
   </si>
 </sst>
 </file>
@@ -773,11 +770,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D2D1F1-7BA5-4534-88B6-D969E332B0E1}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1071,9 +1066,7 @@
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>51</v>
       </c>
@@ -1100,25 +1093,27 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="M9" s="3"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1131,29 +1126,25 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1166,7 +1157,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>40</v>
@@ -1177,7 +1168,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1185,7 +1176,9 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
@@ -1194,39 +1187,6 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>